<commit_message>
Changed the Effort-Estimation Date
</commit_message>
<xml_diff>
--- a/EffortEstimation/4 Weeks Estimation.xlsx
+++ b/EffortEstimation/4 Weeks Estimation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Schule\SYP\Allround Manager\project-proposal-allround-manager-prototype-name\EffortEstimation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A311FF2-4049-4EC8-BAF8-B4A1D7438FBD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48BFF75-35AE-4AC5-B586-3D2F9BC260D5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="345" windowWidth="19815" windowHeight="12060" xr2:uid="{A86B2A40-5864-4E44-B1D9-9A99AF58399A}"/>
+    <workbookView xWindow="3780" yWindow="3255" windowWidth="19815" windowHeight="12060" xr2:uid="{A86B2A40-5864-4E44-B1D9-9A99AF58399A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="31">
   <si>
     <t>Task</t>
   </si>
@@ -63,18 +63,6 @@
     <t>1h</t>
   </si>
   <si>
-    <t>Woche 2 until 26.03.2019</t>
-  </si>
-  <si>
-    <t>Woche 3 until 02.04.2019</t>
-  </si>
-  <si>
-    <t>Woche 4 until 11.04.2019</t>
-  </si>
-  <si>
-    <t>Woche 1 until 19.03.2019</t>
-  </si>
-  <si>
     <t>Data safed on local Data base</t>
   </si>
   <si>
@@ -124,13 +112,25 @@
   </si>
   <si>
     <t>Data safed on local data base</t>
+  </si>
+  <si>
+    <t>Woche 1 until 21.03.2019</t>
+  </si>
+  <si>
+    <t>Woche 2 until 28.03.2019</t>
+  </si>
+  <si>
+    <t>Woche 3 until 04.04.2019</t>
+  </si>
+  <si>
+    <t>Woche 4 until 13.04.2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,8 +146,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,6 +172,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -179,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -195,6 +207,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -513,7 +534,7 @@
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,8 +572,8 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
+      <c r="A4" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -577,7 +598,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>8</v>
@@ -585,13 +606,13 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>6</v>
@@ -599,13 +620,13 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>8</v>
@@ -613,7 +634,7 @@
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F10" s="5"/>
     </row>
@@ -664,8 +685,8 @@
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>10</v>
+      <c r="A17" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -690,7 +711,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>7</v>
@@ -698,27 +719,27 @@
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>8</v>
@@ -726,13 +747,13 @@
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>9</v>
@@ -740,7 +761,7 @@
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F24" s="5"/>
     </row>
@@ -753,8 +774,8 @@
       <c r="F25" s="5"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>11</v>
+      <c r="A29" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -800,7 +821,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>6</v>
@@ -808,13 +829,13 @@
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>8</v>
@@ -822,24 +843,24 @@
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>12</v>
+      <c r="A42" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -885,7 +906,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>6</v>
@@ -893,21 +914,21 @@
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F46" s="5"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F47" s="5"/>
     </row>

</xml_diff>